<commit_message>
Finished the report creator tool
</commit_message>
<xml_diff>
--- a/Python/excel_automation/data.xlsx
+++ b/Python/excel_automation/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t xml:space="preserve">Abraof plays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken gun rooster rudy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tio chico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pitsecato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fortfire leaks</t>
   </si>
 </sst>
 </file>
@@ -332,15 +350,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,10 +409,10 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>39821</v>
       </c>
     </row>
@@ -402,10 +420,10 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>3213</v>
       </c>
     </row>
@@ -413,10 +431,10 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>5000</v>
       </c>
     </row>
@@ -424,10 +442,10 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>8512</v>
       </c>
     </row>
@@ -435,11 +453,66 @@
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>2315</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>312358</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>